<commit_message>
BATAU - TemplateUpdate Category KPIs
</commit_message>
<xml_diff>
--- a/Projects/BATAU/Data/Template.xlsx
+++ b/Projects/BATAU/Data/Template.xlsx
@@ -440,23 +440,23 @@
   <dimension ref="1:27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.2914979757085"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="43.6882591093117"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.2753036437247"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.5060728744939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.3684210526316"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="12.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="69.9352226720648"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.6801619433198"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="47.5546558704454"/>
-    <col collapsed="false" hidden="false" max="1020" min="11" style="2" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="44.668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="71.663967611336"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="1020" min="11" style="2" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1303,7 +1303,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>54</v>
@@ -1340,18 +1340,18 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="1" sqref="E27 E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.53441295546559"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="71.0202429149798"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.9473684210526"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="48.417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.5951417004049"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="3.53441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
@@ -1432,7 +1432,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E27 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1458,7 +1458,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E27 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
BATAU - kpis update
</commit_message>
<xml_diff>
--- a/Projects/BATAU/Data/Template.xlsx
+++ b/Projects/BATAU/Data/Template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="118">
   <si>
     <t xml:space="preserve">kpi_parent_name</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve">BAT_SOR_All_Manf_All_Brands_Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOR-Brand</t>
   </si>
   <si>
     <t xml:space="preserve">manufacturer_name,brand_name</t>
@@ -613,22 +616,22 @@
   </sheetPr>
   <dimension ref="1:57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="54.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.9554655870445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="54.7368421052632"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="40.7044534412955"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="105.085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="80.4453441295547"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="41.0283400809717"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="106.048582995951"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="81.1943319838057"/>
     <col collapsed="false" hidden="false" max="1020" min="11" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1021" style="1" width="9.10526315789474"/>
   </cols>
@@ -23688,7 +23691,7 @@
         <v>11</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>33</v>
@@ -23697,12 +23700,12 @@
         <v>13</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J24" s="7" t="s">
@@ -23716,28 +23719,28 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6"/>
       <c r="B25" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>16</v>
@@ -23745,31 +23748,31 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>16</v>
@@ -23777,31 +23780,31 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>16</v>
@@ -23810,941 +23813,941 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G28" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="J28" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
       <c r="B29" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="J29" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G30" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="J30" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
       <c r="B31" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="J31" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
       <c r="B32" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G32" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="J32" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
       <c r="B33" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G33" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H33" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="J33" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
       <c r="B34" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G34" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I34" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="J34" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
       <c r="B35" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G35" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I35" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="J35" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
       <c r="B36" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G36" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I36" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="J36" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
       <c r="B37" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G37" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I37" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="J37" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -24771,13 +24774,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.53441295546559"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.2348178137652"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8744939271255"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="50.3441295546559"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="50.7732793522267"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="3.53441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
@@ -24789,54 +24792,54 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>